<commit_message>
Cambios, en comprobante e ingresos
</commit_message>
<xml_diff>
--- a/Ejemplo Recibo.xlsx
+++ b/Ejemplo Recibo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VisualStudio\Personal\Roberto-Conjuntos\ProyectoConjuntos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VisualS\ProyectoConjuntos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E5DC73-8C07-4DA4-BBF0-41E4FFDC8A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9CBD42-A62C-4389-9159-862660ECCEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{22DC33CE-D425-4658-B823-985CC8883F2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22DC33CE-D425-4658-B823-985CC8883F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
   <si>
     <t>Número departamento</t>
   </si>
@@ -93,9 +104,6 @@
     <t>Todos</t>
   </si>
   <si>
-    <t>Recibo</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -111,9 +119,6 @@
     <t>Mes de marzo 2024</t>
   </si>
   <si>
-    <t>Forma de pago</t>
-  </si>
-  <si>
     <t>Recibi Conforme</t>
   </si>
   <si>
@@ -126,9 +131,6 @@
     <t>Saldo</t>
   </si>
   <si>
-    <t>Efectivo, Transferencia, Cheque</t>
-  </si>
-  <si>
     <t>Guardar</t>
   </si>
   <si>
@@ -139,6 +141,78 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Banco</t>
+  </si>
+  <si>
+    <t>Recibo Ingreso</t>
+  </si>
+  <si>
+    <t>Pinchincha, Internacional, Caja, caja general</t>
+  </si>
+  <si>
+    <t>Cuenta</t>
+  </si>
+  <si>
+    <t>Detalle</t>
+  </si>
+  <si>
+    <t>Debito</t>
+  </si>
+  <si>
+    <t>Crédito</t>
+  </si>
+  <si>
+    <t>Credito</t>
+  </si>
+  <si>
+    <t>490,32 (cuando se genera el adeudo)</t>
+  </si>
+  <si>
+    <t>Cuando se Genra el adeudo, individual mente</t>
+  </si>
+  <si>
+    <t>Cuando se genera el ingreso</t>
+  </si>
+  <si>
+    <t>1.1.02.01 BANCO PICHINHA</t>
+  </si>
+  <si>
+    <t>1.1.03.01 ADEUDOS ORDINARIOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1.01.01 Ingreso Expensas </t>
+  </si>
+  <si>
+    <t>Pago de Enero</t>
+  </si>
+  <si>
+    <t>Condomino</t>
+  </si>
+  <si>
+    <t>Torre 1 - 102</t>
+  </si>
+  <si>
+    <t>Torre 2 - 201</t>
+  </si>
+  <si>
+    <t>Pago de Enero, Febrero y marzo</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t># Documento</t>
+  </si>
+  <si>
+    <t>Registro interno del sistema</t>
+  </si>
+  <si>
+    <t>1.1.02.01 BANCO PICHINHA (Consulta del mayor por cuenta y po rango de fechas)</t>
   </si>
 </sst>
 </file>
@@ -178,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,8 +265,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -523,11 +609,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -576,35 +745,111 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,326 +1184,690 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6876C447-EB89-45A1-898A-4725254FCB86}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" customWidth="1"/>
+    <col min="10" max="10" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="41"/>
+    </row>
+    <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="4"/>
+      <c r="J2" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>105</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4"/>
+      <c r="K4" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="4"/>
+      <c r="E5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="38"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="G2" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>105</v>
-      </c>
-      <c r="G3" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-    </row>
-    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="H4" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-    </row>
-    <row r="5" spans="1:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4"/>
-      <c r="C5" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="32"/>
-    </row>
-    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="38"/>
+    </row>
+    <row r="6" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="8"/>
-      <c r="J6" s="4"/>
-      <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J7" s="11" t="s">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="8"/>
+      <c r="M6" s="4"/>
+      <c r="S6" s="5"/>
+    </row>
+    <row r="7" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7">
+        <v>105</v>
+      </c>
+      <c r="S7" s="5"/>
+    </row>
+    <row r="8" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="27"/>
+      <c r="I8" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="S8" s="5"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="53"/>
+      <c r="E9" s="21">
+        <v>105</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="21">
+        <v>50</v>
+      </c>
+      <c r="H9" s="21"/>
+      <c r="I9" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" s="4"/>
+      <c r="S9" s="5"/>
+    </row>
+    <row r="10" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="54"/>
+      <c r="E10" s="22">
+        <v>105</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="22">
+        <v>50</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="4"/>
+      <c r="S10" s="5"/>
+    </row>
+    <row r="11" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="55"/>
+      <c r="E11" s="23">
+        <v>105</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="23">
+        <v>50</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="N7">
-        <v>105</v>
-      </c>
-      <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="29" t="s">
+      <c r="N11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11">
+        <v>50</v>
+      </c>
+      <c r="R11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="S11" s="30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="M12" s="4"/>
+      <c r="N12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12">
+        <v>50</v>
+      </c>
+      <c r="S12" s="5"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>80</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="P13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>100</v>
+      </c>
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="M14" s="4"/>
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="M15" s="4"/>
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I16" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="I17" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="45"/>
+      <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="21">
-        <v>105</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="21">
+      <c r="O17" t="s">
+        <v>37</v>
+      </c>
+      <c r="S17" s="5"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="4"/>
-      <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="22">
-        <v>105</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="22">
+      <c r="E18" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="68"/>
+      <c r="I18" s="49">
+        <v>34.79</v>
+      </c>
+      <c r="J18" s="43"/>
+      <c r="M18" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="S18" s="5"/>
+    </row>
+    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="63">
+        <v>34.79</v>
+      </c>
+      <c r="F19" s="62"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="57">
+        <v>104.37</v>
+      </c>
+      <c r="J19" s="44"/>
+      <c r="M19" s="4"/>
+      <c r="S19" s="5"/>
+    </row>
+    <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61">
+        <v>34.79</v>
+      </c>
+      <c r="G20" s="52"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="44"/>
+      <c r="M20" s="4"/>
+      <c r="N20" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S20" s="5"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="60"/>
+      <c r="C21" s="58" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59">
+        <f>SUM(E19:E20)</f>
+        <v>34.79</v>
+      </c>
+      <c r="F21" s="59">
+        <f>SUM(F20)</f>
+        <v>34.79</v>
+      </c>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="M21" s="4"/>
+      <c r="S21" s="5"/>
+    </row>
+    <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="8"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="61">
+        <f>E19*3</f>
+        <v>104.37</v>
+      </c>
+      <c r="F23" s="60"/>
+      <c r="I23" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61">
+        <f>E23</f>
+        <v>104.37</v>
+      </c>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+    </row>
+    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="60"/>
+      <c r="C25" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59">
+        <f>SUM(E23:E24)</f>
+        <v>104.37</v>
+      </c>
+      <c r="F25" s="59">
+        <f>SUM(F24)</f>
+        <v>104.37</v>
+      </c>
+      <c r="I25" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="45"/>
+    </row>
+    <row r="26" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="71"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="50"/>
+      <c r="I26" s="51">
+        <v>490.32</v>
+      </c>
+      <c r="J26" s="48">
+        <v>34.79</v>
+      </c>
+      <c r="K26" s="52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="78"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="69">
+        <v>104.37</v>
+      </c>
+      <c r="K27" s="52"/>
+    </row>
+    <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="67" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="67" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="23">
-        <v>105</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="23">
-        <v>50</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N11">
-        <v>50</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="P11" s="34">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J12" s="4"/>
-      <c r="K12" t="s">
+      <c r="E28" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="N12">
-        <v>50</v>
-      </c>
-      <c r="P12" s="5"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G13">
-        <v>80</v>
-      </c>
-      <c r="J13" s="4"/>
-      <c r="M13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N13" s="10">
-        <v>100</v>
-      </c>
-      <c r="P13" s="5"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J14" s="4"/>
-      <c r="P14" s="5"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J15" s="4"/>
-      <c r="P15" s="5"/>
-    </row>
-    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J16" s="4"/>
-      <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J17" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L17" t="s">
-        <v>33</v>
-      </c>
-      <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J18" s="4"/>
-      <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J19" s="4"/>
-      <c r="P19" s="5"/>
-    </row>
-    <row r="20" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J20" s="4"/>
-      <c r="K20" t="s">
-        <v>29</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P20" s="5"/>
-    </row>
-    <row r="21" spans="10:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J21" s="6"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="8"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="52">
+        <f>I26-J26</f>
+        <v>455.53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="76">
+        <v>45455</v>
+      </c>
+      <c r="B29" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="63">
+        <v>1212</v>
+      </c>
+      <c r="D29" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="63">
+        <v>34.79</v>
+      </c>
+      <c r="F29" s="63">
+        <v>0</v>
+      </c>
+      <c r="G29" s="62">
+        <f>E29-F29</f>
+        <v>34.79</v>
+      </c>
+      <c r="H29" s="42"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="75">
+        <v>45455</v>
+      </c>
+      <c r="B30" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="61">
+        <v>45453</v>
+      </c>
+      <c r="D30" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="61">
+        <f>E29*3</f>
+        <v>104.37</v>
+      </c>
+      <c r="F30" s="61">
+        <v>0</v>
+      </c>
+      <c r="G30" s="60">
+        <f>G29+E30-F30</f>
+        <v>139.16</v>
+      </c>
+      <c r="H30" s="42"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="60"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="J31" s="42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="60"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="J32" s="45"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="60"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="60"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="44"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="60"/>
+      <c r="B35" s="74"/>
+      <c r="C35" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="58"/>
+      <c r="E35" s="59">
+        <f>SUM(E29:E34)</f>
+        <v>139.16</v>
+      </c>
+      <c r="F35" s="59">
+        <f>SUM(F29:F34)</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="60"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="J5:P5"/>
-    <mergeCell ref="A1:H1"/>
+  <mergeCells count="10">
+    <mergeCell ref="M5:S5"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="K26:K28"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="A27:G27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correciones: ordenamiento de listas, creación de condomino individual
</commit_message>
<xml_diff>
--- a/Ejemplo Recibo.xlsx
+++ b/Ejemplo Recibo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VisualS\ProyectoConjuntos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual\ProyectoConjuntos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9CBD42-A62C-4389-9159-862660ECCEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4162FB3-8219-4AE6-9610-3987BD1C7358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22DC33CE-D425-4658-B823-985CC8883F2F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22DC33CE-D425-4658-B823-985CC8883F2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Número departamento</t>
   </si>
@@ -213,6 +213,12 @@
   </si>
   <si>
     <t>1.1.02.01 BANCO PICHINHA (Consulta del mayor por cuenta y po rango de fechas)</t>
+  </si>
+  <si>
+    <t>TIPO PAGO RECIBO</t>
+  </si>
+  <si>
+    <t>TPRECIB</t>
   </si>
 </sst>
 </file>
@@ -696,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -755,30 +761,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -795,18 +779,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -827,25 +805,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1186,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6876C447-EB89-45A1-898A-4725254FCB86}">
   <dimension ref="A1:S35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1207,18 +1206,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="41"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="70"/>
     </row>
     <row r="2" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4"/>
@@ -1260,15 +1259,15 @@
       <c r="K5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="36" t="s">
+      <c r="M5" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="38"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="67"/>
     </row>
     <row r="6" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
@@ -1332,7 +1331,7 @@
       <c r="C9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="53"/>
+      <c r="D9" s="45"/>
       <c r="E9" s="21">
         <v>105</v>
       </c>
@@ -1359,7 +1358,7 @@
       <c r="C10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="54"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="22">
         <v>105</v>
       </c>
@@ -1389,7 +1388,7 @@
       <c r="C11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="55"/>
+      <c r="D11" s="47"/>
       <c r="E11" s="23">
         <v>105</v>
       </c>
@@ -1463,27 +1462,27 @@
       <c r="S15" s="5"/>
     </row>
     <row r="16" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I16" s="42" t="s">
+      <c r="I16" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="42" t="s">
+      <c r="J16" t="s">
         <v>42</v>
       </c>
       <c r="M16" s="4"/>
       <c r="S16" s="5"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="I17" s="45" t="s">
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="I17" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="45"/>
+      <c r="J17" s="71"/>
       <c r="M17" s="11" t="s">
         <v>35</v>
       </c>
@@ -1493,75 +1492,74 @@
       <c r="S17" s="5"/>
     </row>
     <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="54" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="65" t="s">
+      <c r="D18" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="67" t="s">
+      <c r="E18" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="66" t="s">
+      <c r="F18" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="52" t="s">
+      <c r="G18" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="H18" s="68"/>
-      <c r="I18" s="49">
+      <c r="H18" s="44"/>
+      <c r="I18" s="41">
         <v>34.79</v>
       </c>
-      <c r="J18" s="43"/>
-      <c r="M18" s="70" t="s">
+      <c r="J18" s="36"/>
+      <c r="M18" s="59" t="s">
         <v>56</v>
       </c>
       <c r="S18" s="5"/>
     </row>
     <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="63">
+      <c r="E19" s="53">
         <v>34.79</v>
       </c>
-      <c r="F19" s="62"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="57">
+      <c r="F19" s="52"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="3">
         <v>104.37</v>
       </c>
-      <c r="J19" s="44"/>
+      <c r="J19" s="37"/>
       <c r="M19" s="4"/>
       <c r="S19" s="5"/>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61">
+      <c r="E20" s="51"/>
+      <c r="F20" s="51">
         <v>34.79</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="44"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="44"/>
+      <c r="J20" s="37"/>
       <c r="M20" s="4"/>
       <c r="N20" t="s">
         <v>27</v>
@@ -1572,34 +1570,30 @@
       <c r="S20" s="5"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="60"/>
-      <c r="C21" s="58" t="s">
+      <c r="B21" s="50"/>
+      <c r="C21" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="58"/>
-      <c r="E21" s="59">
+      <c r="D21" s="48"/>
+      <c r="E21" s="49">
         <f>SUM(E19:E20)</f>
         <v>34.79</v>
       </c>
-      <c r="F21" s="59">
+      <c r="F21" s="49">
         <f>SUM(F20)</f>
         <v>34.79</v>
       </c>
-      <c r="G21" s="68"/>
-      <c r="H21" s="68"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
       <c r="M21" s="4"/>
       <c r="S21" s="5"/>
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
       <c r="M22" s="6"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
@@ -1609,252 +1603,245 @@
       <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="61">
+      <c r="E23" s="51">
         <f>E19*3</f>
         <v>104.37</v>
       </c>
-      <c r="F23" s="60"/>
-      <c r="I23" s="42" t="s">
+      <c r="F23" s="50"/>
+      <c r="I23" t="s">
         <v>40</v>
       </c>
-      <c r="J23" s="42" t="s">
+      <c r="J23" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61">
+      <c r="E24" s="51"/>
+      <c r="F24" s="51">
         <f>E23</f>
         <v>104.37</v>
       </c>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
     </row>
     <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="60"/>
-      <c r="C25" s="58" t="s">
+      <c r="B25" s="50"/>
+      <c r="C25" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="58"/>
-      <c r="E25" s="59">
+      <c r="D25" s="48"/>
+      <c r="E25" s="49">
         <f>SUM(E23:E24)</f>
         <v>104.37</v>
       </c>
-      <c r="F25" s="59">
+      <c r="F25" s="49">
         <f>SUM(F24)</f>
         <v>104.37</v>
       </c>
-      <c r="I25" s="45" t="s">
+      <c r="I25" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="J25" s="45"/>
+      <c r="J25" s="71"/>
+      <c r="N25" t="s">
+        <v>59</v>
+      </c>
+      <c r="P25" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="26" spans="1:19" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="71"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="50" t="s">
+      <c r="G26" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="50"/>
-      <c r="I26" s="51">
+      <c r="H26" s="42"/>
+      <c r="I26" s="43">
         <v>490.32</v>
       </c>
-      <c r="J26" s="48">
+      <c r="J26" s="40">
         <v>34.79</v>
       </c>
-      <c r="K26" s="52" t="s">
+      <c r="K26" s="72" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="78" t="s">
+      <c r="A27" s="75" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="78"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="78"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="69">
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="J27" s="58">
         <v>104.37</v>
       </c>
-      <c r="K27" s="52"/>
+      <c r="K27" s="72"/>
     </row>
     <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="67" t="s">
+      <c r="A28" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="77" t="s">
+      <c r="D28" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="67" t="s">
+      <c r="E28" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="66" t="s">
+      <c r="F28" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="G28" s="67" t="s">
+      <c r="G28" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="56"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="52">
+      <c r="H28" s="9"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="72">
         <f>I26-J26</f>
         <v>455.53</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="76">
+      <c r="A29" s="63">
         <v>45455</v>
       </c>
-      <c r="B29" s="73" t="s">
+      <c r="B29" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="63">
+      <c r="C29" s="53">
         <v>1212</v>
       </c>
-      <c r="D29" s="62" t="s">
+      <c r="D29" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="63">
+      <c r="E29" s="53">
         <v>34.79</v>
       </c>
-      <c r="F29" s="63">
+      <c r="F29" s="53">
         <v>0</v>
       </c>
-      <c r="G29" s="62">
+      <c r="G29" s="52">
         <f>E29-F29</f>
         <v>34.79</v>
       </c>
-      <c r="H29" s="42"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="75">
+      <c r="A30" s="62">
         <v>45455</v>
       </c>
-      <c r="B30" s="74" t="s">
+      <c r="B30" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="61">
+      <c r="C30" s="51">
         <v>45453</v>
       </c>
-      <c r="D30" s="60" t="s">
+      <c r="D30" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E30" s="61">
+      <c r="E30" s="51">
         <f>E29*3</f>
         <v>104.37</v>
       </c>
-      <c r="F30" s="61">
+      <c r="F30" s="51">
         <v>0</v>
       </c>
-      <c r="G30" s="60">
+      <c r="G30" s="50">
         <f>G29+E30-F30</f>
         <v>139.16</v>
       </c>
-      <c r="H30" s="42"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="60"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42" t="s">
+      <c r="A31" s="50"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="49"/>
+      <c r="F31" s="49"/>
+      <c r="G31" s="50"/>
+      <c r="I31" t="s">
         <v>40</v>
       </c>
-      <c r="J31" s="42" t="s">
+      <c r="J31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="60"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="45" t="s">
+      <c r="A32" s="50"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="50"/>
+      <c r="I32" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J32" s="45"/>
+      <c r="J32" s="71"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="60"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="60"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="47" t="s">
+      <c r="A33" s="50"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="50"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="39" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="60"/>
-      <c r="B34" s="74"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="44"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="50"/>
+      <c r="J34" s="37"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="60"/>
-      <c r="B35" s="74"/>
-      <c r="C35" s="58" t="s">
+      <c r="A35" s="50"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="58"/>
-      <c r="E35" s="59">
+      <c r="D35" s="48"/>
+      <c r="E35" s="49">
         <f>SUM(E29:E34)</f>
         <v>139.16</v>
       </c>
-      <c r="F35" s="59">
+      <c r="F35" s="49">
         <f>SUM(F29:F34)</f>
         <v>0</v>
       </c>
-      <c r="G35" s="60"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="44"/>
+      <c r="G35" s="50"/>
+      <c r="J35" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>